<commit_message>
20.08.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/August/Others/Distributor & DSR wise Sales target -Rajshahi-August,2020.xlsx
+++ b/2020/August/Others/Distributor & DSR wise Sales target -Rajshahi-August,2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Distributor Primary" sheetId="1" r:id="rId1"/>
@@ -1037,7 +1037,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1186,6 +1186,14 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1213,14 +1221,21 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="10" fillId="8" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1630,7 +1645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1643,7 +1658,7 @@
   </sheetPr>
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -2568,115 +2583,115 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:36" s="74" customFormat="1">
-      <c r="A10" s="71" t="s">
+    <row r="10" spans="1:36" s="65" customFormat="1">
+      <c r="A10" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="73">
+      <c r="C10" s="64">
         <f t="shared" si="0"/>
         <v>6342325.6663619038</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="64">
         <f t="shared" si="1"/>
         <v>4010</v>
       </c>
-      <c r="E10" s="73">
+      <c r="E10" s="64">
         <v>274</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="64">
         <v>328</v>
       </c>
-      <c r="G10" s="73">
+      <c r="G10" s="64">
         <v>328</v>
       </c>
-      <c r="H10" s="73">
+      <c r="H10" s="64">
         <v>95</v>
       </c>
-      <c r="I10" s="73">
+      <c r="I10" s="64">
         <v>180</v>
       </c>
-      <c r="J10" s="73">
+      <c r="J10" s="64">
         <v>159</v>
       </c>
-      <c r="K10" s="73">
+      <c r="K10" s="64">
         <v>307</v>
       </c>
-      <c r="L10" s="73">
+      <c r="L10" s="64">
         <v>190</v>
       </c>
-      <c r="M10" s="73">
+      <c r="M10" s="64">
         <v>222</v>
       </c>
-      <c r="N10" s="73">
+      <c r="N10" s="64">
         <v>180</v>
       </c>
-      <c r="O10" s="73">
+      <c r="O10" s="64">
         <v>95</v>
       </c>
-      <c r="P10" s="73">
+      <c r="P10" s="64">
         <v>265</v>
       </c>
-      <c r="Q10" s="73">
+      <c r="Q10" s="64">
         <v>137</v>
       </c>
-      <c r="R10" s="73">
+      <c r="R10" s="64">
         <v>180</v>
       </c>
-      <c r="S10" s="73">
+      <c r="S10" s="64">
         <v>137</v>
       </c>
-      <c r="T10" s="73">
+      <c r="T10" s="64">
         <v>137</v>
       </c>
-      <c r="U10" s="73">
+      <c r="U10" s="64">
         <v>98</v>
       </c>
-      <c r="V10" s="73">
+      <c r="V10" s="64">
         <v>137</v>
       </c>
-      <c r="W10" s="73">
+      <c r="W10" s="64">
         <v>65</v>
       </c>
-      <c r="X10" s="73">
+      <c r="X10" s="64">
         <v>5</v>
       </c>
-      <c r="Y10" s="73">
+      <c r="Y10" s="64">
         <v>17</v>
       </c>
-      <c r="Z10" s="73">
+      <c r="Z10" s="64">
         <v>15</v>
       </c>
-      <c r="AA10" s="73">
+      <c r="AA10" s="64">
         <v>64</v>
       </c>
-      <c r="AB10" s="73">
+      <c r="AB10" s="64">
         <v>12</v>
       </c>
-      <c r="AC10" s="73">
+      <c r="AC10" s="64">
         <v>64</v>
       </c>
-      <c r="AD10" s="73">
+      <c r="AD10" s="64">
         <v>15</v>
       </c>
-      <c r="AE10" s="73">
+      <c r="AE10" s="64">
         <v>33</v>
       </c>
-      <c r="AF10" s="73">
+      <c r="AF10" s="64">
         <v>47</v>
       </c>
-      <c r="AG10" s="73">
+      <c r="AG10" s="64">
         <v>85</v>
       </c>
-      <c r="AH10" s="73">
+      <c r="AH10" s="64">
         <v>42</v>
       </c>
-      <c r="AI10" s="73">
+      <c r="AI10" s="64">
         <v>59</v>
       </c>
-      <c r="AJ10" s="73">
+      <c r="AJ10" s="64">
         <v>38</v>
       </c>
     </row>
@@ -3128,227 +3143,227 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:36" s="74" customFormat="1">
-      <c r="A15" s="71" t="s">
+    <row r="15" spans="1:36" s="65" customFormat="1">
+      <c r="A15" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="73">
+      <c r="C15" s="64">
         <f t="shared" si="0"/>
         <v>14984963.159233332</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D15" s="64">
         <f t="shared" si="1"/>
         <v>9123</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="64">
         <v>649</v>
       </c>
-      <c r="F15" s="73">
+      <c r="F15" s="64">
         <v>783</v>
       </c>
-      <c r="G15" s="73">
+      <c r="G15" s="64">
         <v>783</v>
       </c>
-      <c r="H15" s="73">
+      <c r="H15" s="64">
         <v>165</v>
       </c>
-      <c r="I15" s="73">
+      <c r="I15" s="64">
         <v>389</v>
       </c>
-      <c r="J15" s="73">
+      <c r="J15" s="64">
         <v>333</v>
       </c>
-      <c r="K15" s="73">
+      <c r="K15" s="64">
         <v>727</v>
       </c>
-      <c r="L15" s="73">
+      <c r="L15" s="64">
         <v>447</v>
       </c>
-      <c r="M15" s="73">
+      <c r="M15" s="64">
         <v>512</v>
       </c>
-      <c r="N15" s="73">
+      <c r="N15" s="64">
         <v>399</v>
       </c>
-      <c r="O15" s="73">
+      <c r="O15" s="64">
         <v>175</v>
       </c>
-      <c r="P15" s="73">
+      <c r="P15" s="64">
         <v>624</v>
       </c>
-      <c r="Q15" s="73">
+      <c r="Q15" s="64">
         <v>287</v>
       </c>
-      <c r="R15" s="73">
+      <c r="R15" s="64">
         <v>399</v>
       </c>
-      <c r="S15" s="73">
+      <c r="S15" s="64">
         <v>287</v>
       </c>
-      <c r="T15" s="73">
+      <c r="T15" s="64">
         <v>287</v>
       </c>
-      <c r="U15" s="73">
+      <c r="U15" s="64">
         <v>206</v>
       </c>
-      <c r="V15" s="73">
+      <c r="V15" s="64">
         <v>287</v>
       </c>
-      <c r="W15" s="73">
+      <c r="W15" s="64">
         <v>154</v>
       </c>
-      <c r="X15" s="73">
+      <c r="X15" s="64">
         <v>7</v>
       </c>
-      <c r="Y15" s="73">
+      <c r="Y15" s="64">
         <v>38</v>
       </c>
-      <c r="Z15" s="73">
+      <c r="Z15" s="64">
         <v>34</v>
       </c>
-      <c r="AA15" s="73">
+      <c r="AA15" s="64">
         <v>144</v>
       </c>
-      <c r="AB15" s="73">
+      <c r="AB15" s="64">
         <v>26</v>
       </c>
-      <c r="AC15" s="73">
+      <c r="AC15" s="64">
         <v>164</v>
       </c>
-      <c r="AD15" s="73">
+      <c r="AD15" s="64">
         <v>38</v>
       </c>
-      <c r="AE15" s="73">
+      <c r="AE15" s="64">
         <v>85</v>
       </c>
-      <c r="AF15" s="73">
+      <c r="AF15" s="64">
         <v>119</v>
       </c>
-      <c r="AG15" s="73">
+      <c r="AG15" s="64">
         <v>220</v>
       </c>
-      <c r="AH15" s="73">
+      <c r="AH15" s="64">
         <v>107</v>
       </c>
-      <c r="AI15" s="73">
+      <c r="AI15" s="64">
         <v>152</v>
       </c>
-      <c r="AJ15" s="73">
+      <c r="AJ15" s="64">
         <v>96</v>
       </c>
     </row>
-    <row r="16" spans="1:36" s="74" customFormat="1">
-      <c r="A16" s="71" t="s">
+    <row r="16" spans="1:36" s="65" customFormat="1">
+      <c r="A16" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="73">
+      <c r="C16" s="64">
         <f t="shared" si="0"/>
         <v>11738378.345309524</v>
       </c>
-      <c r="D16" s="73">
+      <c r="D16" s="64">
         <f t="shared" si="1"/>
         <v>7311</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="64">
         <v>499</v>
       </c>
-      <c r="F16" s="73">
+      <c r="F16" s="64">
         <v>602</v>
       </c>
-      <c r="G16" s="73">
+      <c r="G16" s="64">
         <v>602</v>
       </c>
-      <c r="H16" s="73">
+      <c r="H16" s="64">
         <v>168</v>
       </c>
-      <c r="I16" s="73">
+      <c r="I16" s="64">
         <v>325</v>
       </c>
-      <c r="J16" s="73">
+      <c r="J16" s="64">
         <v>286</v>
       </c>
-      <c r="K16" s="73">
+      <c r="K16" s="64">
         <v>562</v>
       </c>
-      <c r="L16" s="73">
+      <c r="L16" s="64">
         <v>344</v>
       </c>
-      <c r="M16" s="73">
+      <c r="M16" s="64">
         <v>405</v>
       </c>
-      <c r="N16" s="73">
+      <c r="N16" s="64">
         <v>325</v>
       </c>
-      <c r="O16" s="73">
+      <c r="O16" s="64">
         <v>168</v>
       </c>
-      <c r="P16" s="73">
+      <c r="P16" s="64">
         <v>483</v>
       </c>
-      <c r="Q16" s="73">
+      <c r="Q16" s="64">
         <v>246</v>
       </c>
-      <c r="R16" s="73">
+      <c r="R16" s="64">
         <v>325</v>
       </c>
-      <c r="S16" s="73">
+      <c r="S16" s="64">
         <v>246</v>
       </c>
-      <c r="T16" s="73">
+      <c r="T16" s="64">
         <v>246</v>
       </c>
-      <c r="U16" s="73">
+      <c r="U16" s="64">
         <v>173</v>
       </c>
-      <c r="V16" s="73">
+      <c r="V16" s="64">
         <v>246</v>
       </c>
-      <c r="W16" s="73">
+      <c r="W16" s="64">
         <v>120</v>
       </c>
-      <c r="X16" s="73">
+      <c r="X16" s="64">
         <v>11</v>
       </c>
-      <c r="Y16" s="73">
+      <c r="Y16" s="64">
         <v>30</v>
       </c>
-      <c r="Z16" s="73">
+      <c r="Z16" s="64">
         <v>30</v>
       </c>
-      <c r="AA16" s="73">
+      <c r="AA16" s="64">
         <v>120</v>
       </c>
-      <c r="AB16" s="73">
+      <c r="AB16" s="64">
         <v>24</v>
       </c>
-      <c r="AC16" s="73">
+      <c r="AC16" s="64">
         <v>120</v>
       </c>
-      <c r="AD16" s="73">
+      <c r="AD16" s="64">
         <v>30</v>
       </c>
-      <c r="AE16" s="73">
+      <c r="AE16" s="64">
         <v>63</v>
       </c>
-      <c r="AF16" s="73">
+      <c r="AF16" s="64">
         <v>88</v>
       </c>
-      <c r="AG16" s="73">
+      <c r="AG16" s="64">
         <v>160</v>
       </c>
-      <c r="AH16" s="73">
+      <c r="AH16" s="64">
         <v>80</v>
       </c>
-      <c r="AI16" s="73">
+      <c r="AI16" s="64">
         <v>112</v>
       </c>
-      <c r="AJ16" s="73">
+      <c r="AJ16" s="64">
         <v>72</v>
       </c>
     </row>
@@ -3913,10 +3928,10 @@
       </c>
     </row>
     <row r="22" spans="1:36">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="62"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="14">
         <f t="shared" si="0"/>
         <v>210711191.60934761</v>
@@ -6350,10 +6365,10 @@
       </c>
     </row>
     <row r="22" spans="1:36">
-      <c r="A22" s="62" t="s">
+      <c r="A22" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="62"/>
+      <c r="B22" s="66"/>
       <c r="C22" s="14">
         <f t="shared" si="0"/>
         <v>215982675</v>
@@ -7629,10 +7644,10 @@
       </c>
     </row>
     <row r="10" spans="1:36">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="62"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="14">
         <f t="shared" si="0"/>
         <v>215982675</v>
@@ -7782,11 +7797,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BA91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7" ySplit="2" topLeftCell="M30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomRight" activeCell="S50" sqref="S50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -7820,25 +7835,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="12.75">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="67" t="s">
         <v>50</v>
       </c>
       <c r="H1" s="6">
@@ -7939,13 +7954,13 @@
       </c>
     </row>
     <row r="2" spans="1:39" ht="12.75">
-      <c r="A2" s="65"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
       <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
@@ -14093,487 +14108,487 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:39">
-      <c r="A53" s="25" t="s">
+    <row r="53" spans="1:39" s="81" customFormat="1">
+      <c r="A53" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="77" t="s">
         <v>133</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E53" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F53" s="78">
         <f t="shared" si="6"/>
         <v>7356715</v>
       </c>
-      <c r="G53" s="26">
+      <c r="G53" s="79">
         <f t="shared" si="7"/>
         <v>4108</v>
       </c>
-      <c r="H53" s="22">
+      <c r="H53" s="80">
         <v>288</v>
       </c>
-      <c r="I53" s="22">
+      <c r="I53" s="80">
         <v>310</v>
       </c>
-      <c r="J53" s="22">
+      <c r="J53" s="80">
         <v>416</v>
       </c>
-      <c r="K53" s="22">
+      <c r="K53" s="80">
         <v>62</v>
       </c>
-      <c r="L53" s="22">
+      <c r="L53" s="80">
         <v>155</v>
       </c>
-      <c r="M53" s="22">
+      <c r="M53" s="80">
         <v>133</v>
       </c>
-      <c r="N53" s="22">
+      <c r="N53" s="80">
         <v>325</v>
       </c>
-      <c r="O53" s="22">
+      <c r="O53" s="80">
         <v>162</v>
       </c>
-      <c r="P53" s="22">
+      <c r="P53" s="80">
         <v>214</v>
       </c>
-      <c r="Q53" s="22">
+      <c r="Q53" s="80">
         <v>178</v>
       </c>
-      <c r="R53" s="22">
+      <c r="R53" s="80">
         <v>70</v>
       </c>
-      <c r="S53" s="22">
+      <c r="S53" s="80">
         <v>256</v>
       </c>
-      <c r="T53" s="22">
+      <c r="T53" s="80">
         <v>139</v>
       </c>
-      <c r="U53" s="22">
+      <c r="U53" s="80">
         <v>178</v>
       </c>
-      <c r="V53" s="22">
+      <c r="V53" s="80">
         <v>116</v>
       </c>
-      <c r="W53" s="22">
+      <c r="W53" s="80">
         <v>146</v>
       </c>
-      <c r="X53" s="22">
+      <c r="X53" s="80">
         <v>84</v>
       </c>
-      <c r="Y53" s="22">
+      <c r="Y53" s="80">
         <v>152</v>
       </c>
-      <c r="Z53" s="22">
+      <c r="Z53" s="80">
         <v>96</v>
       </c>
-      <c r="AA53" s="22">
+      <c r="AA53" s="80">
         <v>4</v>
       </c>
-      <c r="AB53" s="22">
+      <c r="AB53" s="80">
         <v>20</v>
       </c>
-      <c r="AC53" s="22">
+      <c r="AC53" s="80">
         <v>20</v>
       </c>
-      <c r="AD53" s="22">
+      <c r="AD53" s="80">
         <v>79</v>
       </c>
-      <c r="AE53" s="22">
+      <c r="AE53" s="80">
         <v>12</v>
       </c>
-      <c r="AF53" s="22">
+      <c r="AF53" s="80">
         <v>84</v>
       </c>
-      <c r="AG53" s="22">
+      <c r="AG53" s="80">
         <v>16</v>
       </c>
-      <c r="AH53" s="22">
+      <c r="AH53" s="80">
         <v>37</v>
       </c>
-      <c r="AI53" s="22">
+      <c r="AI53" s="80">
         <v>60</v>
       </c>
-      <c r="AJ53" s="22">
+      <c r="AJ53" s="80">
         <v>111</v>
       </c>
-      <c r="AK53" s="22">
+      <c r="AK53" s="80">
         <v>69</v>
       </c>
-      <c r="AL53" s="22">
+      <c r="AL53" s="80">
         <v>69</v>
       </c>
-      <c r="AM53" s="22">
+      <c r="AM53" s="80">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:39">
-      <c r="A54" s="25" t="s">
+    <row r="54" spans="1:39" s="81" customFormat="1">
+      <c r="A54" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="77" t="s">
         <v>135</v>
       </c>
-      <c r="E54" s="25" t="s">
+      <c r="E54" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="78">
         <f t="shared" si="6"/>
         <v>2161845</v>
       </c>
-      <c r="G54" s="26">
+      <c r="G54" s="79">
         <f t="shared" si="7"/>
         <v>1225</v>
       </c>
-      <c r="H54" s="22">
+      <c r="H54" s="80">
         <v>88</v>
       </c>
-      <c r="I54" s="22">
+      <c r="I54" s="80">
         <v>71</v>
       </c>
-      <c r="J54" s="22">
+      <c r="J54" s="80">
         <v>55</v>
       </c>
-      <c r="K54" s="22">
+      <c r="K54" s="80">
         <v>27</v>
       </c>
-      <c r="L54" s="22">
+      <c r="L54" s="80">
         <v>87</v>
       </c>
-      <c r="M54" s="22">
+      <c r="M54" s="80">
         <v>73</v>
       </c>
-      <c r="N54" s="22">
+      <c r="N54" s="80">
         <v>68</v>
       </c>
-      <c r="O54" s="22">
+      <c r="O54" s="80">
         <v>89</v>
       </c>
-      <c r="P54" s="22">
+      <c r="P54" s="80">
         <v>74</v>
       </c>
-      <c r="Q54" s="22">
+      <c r="Q54" s="80">
         <v>36</v>
       </c>
-      <c r="R54" s="22">
+      <c r="R54" s="80">
         <v>24</v>
       </c>
-      <c r="S54" s="22">
+      <c r="S54" s="80">
         <v>106</v>
       </c>
-      <c r="T54" s="22">
+      <c r="T54" s="80">
         <v>32</v>
       </c>
-      <c r="U54" s="22">
+      <c r="U54" s="80">
         <v>77</v>
       </c>
-      <c r="V54" s="22">
+      <c r="V54" s="80">
         <v>35</v>
       </c>
-      <c r="W54" s="22">
+      <c r="W54" s="80">
         <v>34</v>
       </c>
-      <c r="X54" s="22">
+      <c r="X54" s="80">
         <v>35</v>
       </c>
-      <c r="Y54" s="22">
+      <c r="Y54" s="80">
         <v>18</v>
       </c>
-      <c r="Z54" s="22">
+      <c r="Z54" s="80">
         <v>15</v>
       </c>
-      <c r="AA54" s="22">
+      <c r="AA54" s="80">
         <v>1</v>
       </c>
-      <c r="AB54" s="22">
+      <c r="AB54" s="80">
         <v>5</v>
       </c>
-      <c r="AC54" s="22">
+      <c r="AC54" s="80">
         <v>3</v>
       </c>
-      <c r="AD54" s="22">
+      <c r="AD54" s="80">
         <v>8</v>
       </c>
-      <c r="AE54" s="22">
+      <c r="AE54" s="80">
         <v>3</v>
       </c>
-      <c r="AF54" s="22">
+      <c r="AF54" s="80">
         <v>29</v>
       </c>
-      <c r="AG54" s="22">
+      <c r="AG54" s="80">
         <v>6</v>
       </c>
-      <c r="AH54" s="22">
+      <c r="AH54" s="80">
         <v>14</v>
       </c>
-      <c r="AI54" s="22">
+      <c r="AI54" s="80">
         <v>22</v>
       </c>
-      <c r="AJ54" s="22">
+      <c r="AJ54" s="80">
         <v>41</v>
       </c>
-      <c r="AK54" s="22">
+      <c r="AK54" s="80">
         <v>12</v>
       </c>
-      <c r="AL54" s="22">
+      <c r="AL54" s="80">
         <v>21</v>
       </c>
-      <c r="AM54" s="22">
+      <c r="AM54" s="80">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:39">
-      <c r="A55" s="25" t="s">
+    <row r="55" spans="1:39" s="81" customFormat="1">
+      <c r="A55" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D55" s="77" t="s">
         <v>137</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E55" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="78">
         <f t="shared" si="6"/>
         <v>3224208</v>
       </c>
-      <c r="G55" s="26">
+      <c r="G55" s="79">
         <f t="shared" si="7"/>
         <v>2036</v>
       </c>
-      <c r="H55" s="22">
+      <c r="H55" s="80">
         <v>145</v>
       </c>
-      <c r="I55" s="22">
+      <c r="I55" s="80">
         <v>228</v>
       </c>
-      <c r="J55" s="22">
+      <c r="J55" s="80">
         <v>167</v>
       </c>
-      <c r="K55" s="22">
+      <c r="K55" s="80">
         <v>43</v>
       </c>
-      <c r="L55" s="22">
+      <c r="L55" s="80">
         <v>82</v>
       </c>
-      <c r="M55" s="22">
+      <c r="M55" s="80">
         <v>70</v>
       </c>
-      <c r="N55" s="22">
+      <c r="N55" s="80">
         <v>182</v>
       </c>
-      <c r="O55" s="22">
+      <c r="O55" s="80">
         <v>112</v>
       </c>
-      <c r="P55" s="22">
+      <c r="P55" s="80">
         <v>145</v>
       </c>
-      <c r="Q55" s="22">
+      <c r="Q55" s="80">
         <v>101</v>
       </c>
-      <c r="R55" s="22">
+      <c r="R55" s="80">
         <v>36</v>
       </c>
-      <c r="S55" s="22">
+      <c r="S55" s="80">
         <v>131</v>
       </c>
-      <c r="T55" s="22">
+      <c r="T55" s="80">
         <v>58</v>
       </c>
-      <c r="U55" s="22">
+      <c r="U55" s="80">
         <v>41</v>
       </c>
-      <c r="V55" s="22">
+      <c r="V55" s="80">
         <v>50</v>
       </c>
-      <c r="W55" s="22">
+      <c r="W55" s="80">
         <v>54</v>
       </c>
-      <c r="X55" s="22">
+      <c r="X55" s="80">
         <v>44</v>
       </c>
-      <c r="Y55" s="22">
+      <c r="Y55" s="80">
         <v>81</v>
       </c>
-      <c r="Z55" s="22">
+      <c r="Z55" s="80">
         <v>29</v>
       </c>
-      <c r="AA55" s="22">
+      <c r="AA55" s="80">
         <v>1</v>
       </c>
-      <c r="AB55" s="22">
+      <c r="AB55" s="80">
         <v>7</v>
       </c>
-      <c r="AC55" s="22">
+      <c r="AC55" s="80">
         <v>5</v>
       </c>
-      <c r="AD55" s="22">
+      <c r="AD55" s="80">
         <v>36</v>
       </c>
-      <c r="AE55" s="22">
+      <c r="AE55" s="80">
         <v>7</v>
       </c>
-      <c r="AF55" s="22">
+      <c r="AF55" s="80">
         <v>23</v>
       </c>
-      <c r="AG55" s="22">
+      <c r="AG55" s="80">
         <v>11</v>
       </c>
-      <c r="AH55" s="22">
+      <c r="AH55" s="80">
         <v>21</v>
       </c>
-      <c r="AI55" s="22">
+      <c r="AI55" s="80">
         <v>17</v>
       </c>
-      <c r="AJ55" s="22">
+      <c r="AJ55" s="80">
         <v>32</v>
       </c>
-      <c r="AK55" s="22">
+      <c r="AK55" s="80">
         <v>12</v>
       </c>
-      <c r="AL55" s="22">
+      <c r="AL55" s="80">
         <v>44</v>
       </c>
-      <c r="AM55" s="22">
+      <c r="AM55" s="80">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:39">
-      <c r="A56" s="25" t="s">
+    <row r="56" spans="1:39" s="81" customFormat="1">
+      <c r="A56" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B56" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="77" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="25" t="s">
+      <c r="E56" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="78">
         <f t="shared" si="6"/>
         <v>2616857</v>
       </c>
-      <c r="G56" s="26">
+      <c r="G56" s="79">
         <f t="shared" si="7"/>
         <v>1754</v>
       </c>
-      <c r="H56" s="22">
+      <c r="H56" s="80">
         <v>128</v>
       </c>
-      <c r="I56" s="22">
+      <c r="I56" s="80">
         <v>174</v>
       </c>
-      <c r="J56" s="22">
+      <c r="J56" s="80">
         <v>145</v>
       </c>
-      <c r="K56" s="22">
+      <c r="K56" s="80">
         <v>33</v>
       </c>
-      <c r="L56" s="22">
+      <c r="L56" s="80">
         <v>65</v>
       </c>
-      <c r="M56" s="22">
+      <c r="M56" s="80">
         <v>57</v>
       </c>
-      <c r="N56" s="22">
+      <c r="N56" s="80">
         <v>152</v>
       </c>
-      <c r="O56" s="22">
+      <c r="O56" s="80">
         <v>84</v>
       </c>
-      <c r="P56" s="22">
+      <c r="P56" s="80">
         <v>79</v>
       </c>
-      <c r="Q56" s="22">
+      <c r="Q56" s="80">
         <v>84</v>
       </c>
-      <c r="R56" s="22">
+      <c r="R56" s="80">
         <v>45</v>
       </c>
-      <c r="S56" s="22">
+      <c r="S56" s="80">
         <v>131</v>
       </c>
-      <c r="T56" s="22">
+      <c r="T56" s="80">
         <v>58</v>
       </c>
-      <c r="U56" s="22">
+      <c r="U56" s="80">
         <v>103</v>
       </c>
-      <c r="V56" s="22">
+      <c r="V56" s="80">
         <v>86</v>
       </c>
-      <c r="W56" s="22">
+      <c r="W56" s="80">
         <v>53</v>
       </c>
-      <c r="X56" s="22">
+      <c r="X56" s="80">
         <v>43</v>
       </c>
-      <c r="Y56" s="22">
+      <c r="Y56" s="80">
         <v>36</v>
       </c>
-      <c r="Z56" s="22">
+      <c r="Z56" s="80">
         <v>14</v>
       </c>
-      <c r="AA56" s="22">
+      <c r="AA56" s="80">
         <v>1</v>
       </c>
-      <c r="AB56" s="22">
+      <c r="AB56" s="80">
         <v>6</v>
       </c>
-      <c r="AC56" s="22">
+      <c r="AC56" s="80">
         <v>6</v>
       </c>
-      <c r="AD56" s="22">
+      <c r="AD56" s="80">
         <v>21</v>
       </c>
-      <c r="AE56" s="22">
+      <c r="AE56" s="80">
         <v>4</v>
       </c>
-      <c r="AF56" s="22">
+      <c r="AF56" s="80">
         <v>28</v>
       </c>
-      <c r="AG56" s="22">
+      <c r="AG56" s="80">
         <v>5</v>
       </c>
-      <c r="AH56" s="22">
+      <c r="AH56" s="80">
         <v>13</v>
       </c>
-      <c r="AI56" s="22">
+      <c r="AI56" s="80">
         <v>20</v>
       </c>
-      <c r="AJ56" s="22">
+      <c r="AJ56" s="80">
         <v>36</v>
       </c>
-      <c r="AK56" s="22">
+      <c r="AK56" s="80">
         <v>14</v>
       </c>
-      <c r="AL56" s="22">
+      <c r="AL56" s="80">
         <v>18</v>
       </c>
-      <c r="AM56" s="22">
+      <c r="AM56" s="80">
         <v>12</v>
       </c>
     </row>

</xml_diff>